<commit_message>
Modified response code processing
</commit_message>
<xml_diff>
--- a/test/endpoints/configs/get-search-tests.xlsx
+++ b/test/endpoints/configs/get-search-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\yale\clones\lux-middletier\test\endpoints\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB8FFC-3185-430E-B17A-EF4B3CDB0010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2503A895-6204-4A0D-864B-EF7769FDEDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>